<commit_message>
Added Nullable types better support
</commit_message>
<xml_diff>
--- a/samples/Net.Core.Sample/Excels/TableWithHeaders.xlsx
+++ b/samples/Net.Core.Sample/Excels/TableWithHeaders.xlsx
@@ -395,7 +395,7 @@
   <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="B3" sqref="B3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +456,7 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Added Nullable types better support (#2)
* Added Nullable types better support

* Convert winforms sample into .NET 5 porject

* test github action

* Solve issue to github action to build

* Ajust WinForms Aplicaction .NET Version

* change runner to windows

* change project settings
</commit_message>
<xml_diff>
--- a/samples/Net.Core.Sample/Excels/TableWithHeaders.xlsx
+++ b/samples/Net.Core.Sample/Excels/TableWithHeaders.xlsx
@@ -395,7 +395,7 @@
   <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="B3" sqref="B3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +456,7 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>

</xml_diff>